<commit_message>
add foreign table define
</commit_message>
<xml_diff>
--- a/templates/tableStructure.xlsx
+++ b/templates/tableStructure.xlsx
@@ -3,14 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22715"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_2F206C6948C74EE3E979BAFA89738C9863138395" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A99829C6-ECCB-4F4F-A914-26BF3698A63F}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="11_2F206C6948C74EE3E979BAFA89738C9863138395" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{24F89400-0534-4ADA-A20E-7F91799E82A4}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
     <sheet name="FormMaster" sheetId="2" r:id="rId2"/>
+    <sheet name="EXPMaster" sheetId="3" r:id="rId3"/>
+    <sheet name="ENPMaster" sheetId="4" r:id="rId4"/>
+    <sheet name="ENPDetail" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="239">
   <si>
     <t>no</t>
   </si>
@@ -261,6 +267,649 @@
   </si>
   <si>
     <t>datetime</t>
+  </si>
+  <si>
+    <t>回首頁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表格名稱:EXPMaster-費用主檔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系統編號</t>
+  </si>
+  <si>
+    <t>Not Null</t>
+  </si>
+  <si>
+    <t>FormMaster</t>
+  </si>
+  <si>
+    <t>ExpenseKind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>請款類別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.PREPAY-預付款 
+2.PO_STD-驗收請款 
+3.PO_CM_RETURN-退貨折讓 
+4.PO_CM_EXP-一般請款 
+5.NPO_CM_EXP-一般折讓 
+6.NPO_DONATE_EXP-捐贈(贊助)  
+7.EMP_TRAVEL_EXP-出差 
+8.EMP_OTHER_EXP-其他代墊 
+9.EMP_MGR_EXP-經理人交通津貼 
+10.EA_MISC_EXP-雜項請款 
+11.EA_SPECIFIC_EXP-特定用途 
+12.ESP_EXP-一般請款 
+13.ESP_CM_EXP-一般折讓 
+14.ESP_DONATE_EXP-捐贈(贊助)  
+</t>
+  </si>
+  <si>
+    <t>VendorNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>供應商/請款編號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>VendorName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>供應商名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PaymentStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>付款狀態</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.請款審核中
+2.已放行等待付款
+3.已付款</t>
+  </si>
+  <si>
+    <t>Emergency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>急件</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>PayAlone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>單獨付款</t>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EstimatePayDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>預計付款日期</t>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VoucherBeau</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>憑證開立對象</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Books</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>帳務行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>BooksName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>帳務行名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HeaderDesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>請款主旨</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>ExpenseDesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>請款說明</t>
+  </si>
+  <si>
+    <t>VoucherNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商業發票批次序號</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>ApBatchName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>傳票號碼</t>
+  </si>
+  <si>
+    <t>GlDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>總帳日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VendorAddress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>供應商地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VendorKind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>供應商類別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所得人統一編(證號)</t>
+  </si>
+  <si>
+    <t>PermanentPostNum</t>
+  </si>
+  <si>
+    <t>戶籍地址郵遞區號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PermanentAddress</t>
+  </si>
+  <si>
+    <t>戶籍地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ContactPostNum</t>
+  </si>
+  <si>
+    <t>聯絡地址郵遞區號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ContactAddress</t>
+  </si>
+  <si>
+    <t>聯絡地址</t>
+  </si>
+  <si>
+    <t>CertificateKind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>證號別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountryCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>國別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表格名稱:ENPMaster-非請購主檔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>Idx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENPNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非請購單號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ForeignLabor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>購買國外勞務</t>
+  </si>
+  <si>
+    <t>Deduction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所扣</t>
+  </si>
+  <si>
+    <t>Certificate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待補憑證</t>
+  </si>
+  <si>
+    <t>ExpectedDate</t>
+  </si>
+  <si>
+    <t>預計補憑日期</t>
+  </si>
+  <si>
+    <t>Currency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>幣別</t>
+  </si>
+  <si>
+    <t>CurrencyPrecise</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>幣別精確度</t>
+  </si>
+  <si>
+    <t>Rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>匯率</t>
+  </si>
+  <si>
+    <t>decimal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ContractNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合約號碼</t>
+  </si>
+  <si>
+    <t>CertificateKind</t>
+  </si>
+  <si>
+    <t>憑證類別</t>
+  </si>
+  <si>
+    <t>CertificateNum</t>
+  </si>
+  <si>
+    <t>憑證號碼</t>
+  </si>
+  <si>
+    <t>EstimateVoucherDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>憑證日期</t>
+  </si>
+  <si>
+    <t>DiscountInvoice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>折讓發票</t>
+  </si>
+  <si>
+    <t>DiscountInvoiceDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>折讓發票日期</t>
+  </si>
+  <si>
+    <t>DiscountReceive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>折讓收款</t>
+  </si>
+  <si>
+    <t>InvoiceOverdue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>發票逾期說明</t>
+  </si>
+  <si>
+    <t>YearVoucher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跨年度傳票編號</t>
+  </si>
+  <si>
+    <t>BargainingCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>議價編碼</t>
+  </si>
+  <si>
+    <t>CertificateAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>憑證總額 (原幣)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15,6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OriginalAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>憑證稅額（原幣）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TWDAmount</t>
+  </si>
+  <si>
+    <t>金額總計（臺幣）</t>
+  </si>
+  <si>
+    <t>bigint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TWDPayAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稅額總計（臺幣）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PaymentAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>付款金額(臺幣)*</t>
+  </si>
+  <si>
+    <t>bigInt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MARGINAMT</t>
+  </si>
+  <si>
+    <t>付款預扣金額(保證金)</t>
+  </si>
+  <si>
+    <t>WithHoldingAccountingAmount</t>
+  </si>
+  <si>
+    <t>預扣會計項子目(保證金)</t>
+  </si>
+  <si>
+    <t>ExportApplyAttribute</t>
+  </si>
+  <si>
+    <t>匯出申報性質(外幣)</t>
+  </si>
+  <si>
+    <t>表格名稱:ENPDetail-非請購明細檔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>項次</t>
+  </si>
+  <si>
+    <t>identity(1,1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENPMaster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PaymentCategory</t>
+  </si>
+  <si>
+    <t>請款大類</t>
+  </si>
+  <si>
+    <t>PaymentMidCategory</t>
+  </si>
+  <si>
+    <t>請款中類</t>
+  </si>
+  <si>
+    <t>ExpenseAttribute</t>
+  </si>
+  <si>
+    <t>費用屬性</t>
+  </si>
+  <si>
+    <t>AccountingItem</t>
+  </si>
+  <si>
+    <t>會計項子目</t>
+  </si>
+  <si>
+    <t>NeedCertificate</t>
+  </si>
+  <si>
+    <t>需檢附憑證</t>
+  </si>
+  <si>
+    <t>AmortizationFlag</t>
+  </si>
+  <si>
+    <t>攤銷貼標註記</t>
+  </si>
+  <si>
+    <t>OriginalAmount</t>
+  </si>
+  <si>
+    <t>金額（原幣）</t>
+  </si>
+  <si>
+    <t>15,8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OriginalTax</t>
+  </si>
+  <si>
+    <t>稅額（原幣）</t>
+  </si>
+  <si>
+    <t>OriginalSaleAmount</t>
+  </si>
+  <si>
+    <t>銷售額（原幣）</t>
+  </si>
+  <si>
+    <t>金額（臺幣）</t>
+  </si>
+  <si>
+    <t>TWDTax</t>
+  </si>
+  <si>
+    <t>稅額（臺幣）</t>
+  </si>
+  <si>
+    <t>TWDSaleAmount</t>
+  </si>
+  <si>
+    <t>銷售金額（臺幣）</t>
+  </si>
+  <si>
+    <t>AmortizationStartDate</t>
+  </si>
+  <si>
+    <t>攤銷(起)</t>
+  </si>
+  <si>
+    <t>AmortizationEndDate</t>
+  </si>
+  <si>
+    <t>攤銷(迄)</t>
+  </si>
+  <si>
+    <t>IsIncomeDeduction</t>
+  </si>
+  <si>
+    <t>IsCheckCertificate</t>
+  </si>
+  <si>
+    <t>是否須檢附憑證</t>
+  </si>
+  <si>
+    <t>ProjectCategory</t>
+  </si>
+  <si>
+    <t>專案類別</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>專案</t>
+  </si>
+  <si>
+    <t>ProjectItem</t>
+  </si>
+  <si>
+    <t>專案項目</t>
+  </si>
+  <si>
+    <t>VoucherMemo</t>
+  </si>
+  <si>
+    <t>傳票摘要</t>
+  </si>
+  <si>
+    <t>IsDelete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刪除註記</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>DeleteTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表單刪除時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ModifyTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表單修改時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateBy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建立人員工代號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeleteBy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刪除人員工代號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ModifyBy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改人員工代號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -318,7 +967,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +978,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -392,7 +1047,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -421,6 +1076,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -432,6 +1091,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,6 +1113,172 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="非請購"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="8">
+          <cell r="A8"/>
+        </row>
+        <row r="9">
+          <cell r="A9"/>
+        </row>
+        <row r="10">
+          <cell r="A10"/>
+          <cell r="B10"/>
+        </row>
+        <row r="17">
+          <cell r="A17"/>
+        </row>
+        <row r="18">
+          <cell r="A18"/>
+        </row>
+        <row r="19">
+          <cell r="A19"/>
+        </row>
+        <row r="20">
+          <cell r="A20"/>
+        </row>
+        <row r="21">
+          <cell r="A21"/>
+          <cell r="B21"/>
+        </row>
+        <row r="22">
+          <cell r="A22"/>
+          <cell r="B22"/>
+        </row>
+        <row r="23">
+          <cell r="A23"/>
+        </row>
+        <row r="24">
+          <cell r="A24"/>
+        </row>
+        <row r="25">
+          <cell r="A25"/>
+        </row>
+        <row r="26">
+          <cell r="A26"/>
+        </row>
+        <row r="27">
+          <cell r="A27"/>
+        </row>
+        <row r="40">
+          <cell r="A40"/>
+        </row>
+        <row r="41">
+          <cell r="A41"/>
+        </row>
+        <row r="42">
+          <cell r="A42"/>
+        </row>
+        <row r="43">
+          <cell r="A43"/>
+        </row>
+        <row r="44">
+          <cell r="A44"/>
+        </row>
+        <row r="45">
+          <cell r="A45"/>
+          <cell r="B45"/>
+        </row>
+        <row r="46">
+          <cell r="A46"/>
+          <cell r="B46"/>
+        </row>
+        <row r="51">
+          <cell r="A51"/>
+          <cell r="B51"/>
+        </row>
+        <row r="52">
+          <cell r="A52"/>
+          <cell r="B52"/>
+        </row>
+        <row r="53">
+          <cell r="A53"/>
+          <cell r="B53"/>
+        </row>
+        <row r="54">
+          <cell r="A54"/>
+          <cell r="B54"/>
+        </row>
+        <row r="55">
+          <cell r="A55"/>
+          <cell r="B55"/>
+        </row>
+        <row r="56">
+          <cell r="A56"/>
+          <cell r="B56"/>
+        </row>
+        <row r="57">
+          <cell r="A57"/>
+          <cell r="B57"/>
+        </row>
+        <row r="58">
+          <cell r="A58"/>
+          <cell r="B58"/>
+        </row>
+        <row r="59">
+          <cell r="A59"/>
+          <cell r="B59"/>
+        </row>
+        <row r="60">
+          <cell r="A60"/>
+          <cell r="B60"/>
+        </row>
+        <row r="61">
+          <cell r="A61"/>
+          <cell r="B61"/>
+        </row>
+        <row r="62">
+          <cell r="A62"/>
+          <cell r="B62"/>
+        </row>
+        <row r="63">
+          <cell r="A63"/>
+          <cell r="B63"/>
+        </row>
+        <row r="64">
+          <cell r="A64"/>
+          <cell r="B64"/>
+        </row>
+        <row r="65">
+          <cell r="A65"/>
+          <cell r="B65"/>
+        </row>
+        <row r="66">
+          <cell r="A66"/>
+          <cell r="B66"/>
+        </row>
+        <row r="67">
+          <cell r="A67"/>
+          <cell r="B67"/>
+        </row>
+        <row r="68">
+          <cell r="A68"/>
+          <cell r="B68"/>
+        </row>
+        <row r="69">
+          <cell r="A69"/>
+          <cell r="B69"/>
+        </row>
+        <row r="70">
+          <cell r="A70"/>
+          <cell r="B70"/>
+        </row>
+        <row r="71">
+          <cell r="A71"/>
+          <cell r="B71"/>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -781,13 +1612,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5">
-      <c r="A4" s="12">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4"/>
@@ -993,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E53F2B-7222-4EFF-841E-CD5CFB955CAB}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1015,31 +1846,31 @@
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
@@ -1077,291 +1908,291 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="47.25">
-      <c r="A4" s="12">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="14">
         <v>4</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
       <c r="K4" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="299.25">
-      <c r="A5" s="12">
+      <c r="A5" s="14">
         <v>2</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="14">
         <v>4</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
       <c r="J5" s="11" t="s">
         <v>30</v>
       </c>
       <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="12">
+      <c r="A6" s="14">
         <v>3</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="14">
         <v>10</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="12">
+      <c r="A7" s="14">
         <v>4</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="14">
         <v>20</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="12">
+      <c r="A8" s="14">
         <v>5</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="14">
         <v>10</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="12">
+      <c r="A9" s="14">
         <v>6</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="14">
         <v>10</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="12">
+      <c r="A10" s="14">
         <v>7</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="14">
         <v>20</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="12">
+      <c r="A11" s="14">
         <v>8</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="14">
         <v>10</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A12" s="12">
+      <c r="A12" s="14">
         <v>9</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="14">
         <v>30</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" ht="110.25">
-      <c r="A13" s="12">
+      <c r="A13" s="14">
         <v>10</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="14">
         <v>4</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12" t="s">
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="13"/>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="12">
+      <c r="A14" s="14">
         <v>11</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="14">
         <v>8</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12" t="s">
+      <c r="G14" s="14"/>
+      <c r="H14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="12">
+      <c r="A15" s="14">
         <v>12</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="14">
         <v>8</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="4"/>
     </row>
   </sheetData>
@@ -1373,4 +2204,2117 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D707C6-5111-4B3C-862E-EBB432075156}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="3" max="3" width="21.875" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
+    <col min="7" max="7" width="17.875" customWidth="1"/>
+    <col min="8" max="8" width="18.125" customWidth="1"/>
+    <col min="9" max="9" width="30.125" customWidth="1"/>
+    <col min="10" max="10" width="30.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" s="12" customFormat="1">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="14">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="14">
+        <v>4</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="122.25" customHeight="1">
+      <c r="A5" s="14">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="31.5">
+      <c r="A6" s="14">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" ht="31.5">
+      <c r="A7" s="14">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="14">
+        <v>100</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="47.25">
+      <c r="A8" s="14">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="14">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="14">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="14">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="14">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="14">
+        <v>3</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="14">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="14">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="14">
+        <v>50</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="14">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="14">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="14">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="14">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="14">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="14">
+        <v>3</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="14">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="14">
+        <v>500</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="14">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="14">
+        <v>20</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A22" s="14">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="14">
+        <v>30</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" ht="31.5">
+      <c r="A23" s="14">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="14">
+        <v>10</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="14">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="14">
+        <v>500</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="31.5">
+      <c r="A25" s="14">
+        <v>22</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="14">
+        <v>10</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="14">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="14">
+        <v>500</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="14">
+        <v>24</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="14">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="14">
+        <v>25</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="14">
+        <v>10</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Index'!A1" display="回首頁" xr:uid="{9E71DB6D-23AC-45E1-B030-E5200B0EE108}"/>
+    <hyperlink ref="D5" location="'請款類別'!A1" display="請款類別" xr:uid="{FC856144-2302-43CC-8AD1-655150B2A3A6}"/>
+    <hyperlink ref="D6" location="'供應商'!A1" display="供應商" xr:uid="{AA4F8F36-AB12-49EA-B46F-103A32625C99}"/>
+    <hyperlink ref="D8" location="'付款狀態'!A1" display="付款狀態" xr:uid="{62C4E18E-4689-486B-8259-C13426955BC1}"/>
+    <hyperlink ref="D9" location="'急件'!A1" display="急件" xr:uid="{D37597C3-461C-4400-9F7D-7E50A0BE0491}"/>
+    <hyperlink ref="D10" location="'單獨付款'!A1" display="單獨付款" xr:uid="{A7E398EC-3E33-44F3-AB8C-590E243AF0E2}"/>
+    <hyperlink ref="D11" location="'預計付款日期'!A1" display="預計付款日期" xr:uid="{FB5548A1-DF8E-401F-9D48-C064B2D586D9}"/>
+    <hyperlink ref="D12" location="'憑證開立對象'!A1" display="憑證開立對象" xr:uid="{23C7BF75-4739-4C90-83F1-7FF22AECDB6F}"/>
+    <hyperlink ref="D13" location="'帳務行'!A1" display="帳務行" xr:uid="{D4039C92-1C50-4188-AEC7-E0C2761A3720}"/>
+    <hyperlink ref="D15" location="'請款主旨'!A1" display="請款主旨" xr:uid="{2CA9C2C7-151A-42FA-8C60-008331056902}"/>
+    <hyperlink ref="D16" location="'請款說明'!A1" display="請款說明" xr:uid="{0CF51E73-8CE2-4378-8FEC-D4B0F671FB38}"/>
+    <hyperlink ref="D14" location="'帳務行'!A1" display="帳務行" xr:uid="{855DAD3A-05D8-42A5-BE55-70EAFAD7439F}"/>
+    <hyperlink ref="D7" location="'供應商'!A1" display="供應商" xr:uid="{19B30C66-CD03-483D-A2ED-A387C0BAE3CC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6907235-5F8C-4D07-8402-0F5A21A897A9}">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="3" max="3" width="18.125" customWidth="1"/>
+    <col min="4" max="4" width="23.875" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="9" max="9" width="36.875" customWidth="1"/>
+    <col min="10" max="10" width="42.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" s="15" customFormat="1">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="31.5">
+      <c r="A4" s="14">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="14">
+        <v>4</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="14">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="14">
+        <v>20</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="14">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="14">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="14">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="14">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="14">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="14">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="14">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="14">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="14">
+        <v>3</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="14">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="14">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="14">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="14">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="14">
+        <v>20</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="14">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="14">
+        <v>15</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" ht="31.5">
+      <c r="A16" s="14">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="14">
+        <v>3</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="14">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="14">
+        <v>50</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" ht="31.5">
+      <c r="A18" s="14">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="14">
+        <v>3</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="14">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="14">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="14">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="14">
+        <v>2000</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="14">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="14">
+        <v>200</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="14">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="14">
+        <v>50</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="1:10" ht="31.5">
+      <c r="A23" s="14">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="14">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="14">
+        <v>22</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="14">
+        <v>8</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="14">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F26" s="14">
+        <v>8</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" ht="31.5">
+      <c r="A27" s="14">
+        <v>24</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F27" s="14">
+        <v>8</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="14">
+        <v>25</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="31.5">
+      <c r="A29" s="14">
+        <v>26</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" ht="31.5">
+      <c r="A30" s="14">
+        <v>27</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="19">
+        <v>100</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Index'!A1" display="回首頁" xr:uid="{397017FF-C0E2-4993-AF55-85E24FB225B6}"/>
+    <hyperlink ref="D24" location="'金額總計（原幣）'!A1" display="金額總計（原幣）" xr:uid="{06E71E49-76B3-47C7-AEF1-271647FCAD86}"/>
+    <hyperlink ref="D25" location="'金額總計（臺幣）'!A1" display="金額總計（臺幣）" xr:uid="{CB68CC6F-CD9D-4246-875B-E4BB6E0218A0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9C924F-BBAD-4BD4-AE4A-826CE92872E4}">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="24.875" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="17.25" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="16.625" customWidth="1"/>
+    <col min="10" max="10" width="25.125" customWidth="1"/>
+    <col min="11" max="11" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" s="15" customFormat="1">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="14">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="14">
+        <v>4</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="14">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="14">
+        <v>100</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="14">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="14">
+        <v>100</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="14">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="14">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="14">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="14">
+        <v>100</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="14">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="14">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="14">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="14">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="14">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="14">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="14">
+        <v>8</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F14" s="14">
+        <v>8</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="14">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F15" s="14">
+        <v>8</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="14">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F16" s="14">
+        <v>8</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="14">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="14">
+        <v>3</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="14">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="14">
+        <v>3</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="14">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="14">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="14">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="14">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="14">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="14">
+        <v>10</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="14">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="14">
+        <v>20</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="14">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="14">
+        <v>20</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="14">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="14">
+        <v>100</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="14">
+        <v>22</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="14">
+        <v>1</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="14">
+        <v>23</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="14">
+        <v>24</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="14">
+        <v>25</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="14">
+        <v>8</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="14">
+        <v>26</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="14">
+        <v>27</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="14">
+        <v>10</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="14">
+        <v>28</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="14">
+        <v>10</v>
+      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Index'!A1" display="回首頁" xr:uid="{8B8040FA-DAFC-476D-9D26-43136A3B3BB4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>